<commit_message>
En proceso de documentación.
</commit_message>
<xml_diff>
--- a/tb_states77.xlsx
+++ b/tb_states77.xlsx
@@ -19,57 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>names</t>
+    <t>"state"</t>
   </si>
   <si>
-    <t>a</t>
+    <t>"P"</t>
   </si>
   <si>
-    <t>r</t>
+    <t>"V"</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>kl</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>B3</t>
+    <t>"T"</t>
   </si>
 </sst>
 </file>
@@ -387,39 +348,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
@@ -431,18 +383,9 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>9</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
@@ -454,18 +397,9 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
@@ -477,18 +411,9 @@
       <c r="D4">
         <v>7</v>
       </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
@@ -498,20 +423,11 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>8</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>9.66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
@@ -523,18 +439,9 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
@@ -546,19 +453,10 @@
       <c r="D7">
         <v>7</v>
       </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -569,19 +467,10 @@
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9">
         <v>47</v>
@@ -592,42 +481,24 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10">
-        <v>47</v>
+        <v>47.5</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -638,22 +509,13 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>468</v>
+        <v>468.00099999999998</v>
       </c>
       <c r="C12">
         <v>27</v>
@@ -661,19 +523,10 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>6</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -684,19 +537,10 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13">
-        <v>9</v>
-      </c>
-      <c r="F13">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14">
         <v>85</v>
@@ -705,21 +549,12 @@
         <v>73</v>
       </c>
       <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
-      </c>
-      <c r="G14">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15">
         <v>43</v>
@@ -730,19 +565,10 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-      <c r="F15">
-        <v>6</v>
-      </c>
-      <c r="G15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -753,19 +579,10 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>79</v>
-      </c>
-      <c r="G16">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>6</v>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
       </c>
       <c r="B17">
         <v>77</v>
@@ -776,19 +593,10 @@
       <c r="D17">
         <v>9</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>9</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -799,19 +607,10 @@
       <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-      <c r="G18">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19">
         <v>634</v>
@@ -822,19 +621,10 @@
       <c r="D19">
         <v>3</v>
       </c>
-      <c r="E19">
-        <v>5</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>2</v>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -845,19 +635,10 @@
       <c r="D20">
         <v>41</v>
       </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
-      </c>
-      <c r="G20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -867,15 +648,6 @@
       </c>
       <c r="D21">
         <v>3</v>
-      </c>
-      <c r="E21">
-        <v>58</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>